<commit_message>
Atualização: Correção na geração dos arquivos; Taxas Importação subindo para o Supabase; Subindo lastupdate para o supabase e consultando no backend
</commit_message>
<xml_diff>
--- a/app/backend/data/Excel_base/base.xlsx
+++ b/app/backend/data/Excel_base/base.xlsx
@@ -1501,76 +1501,49 @@
     <xf numFmtId="171" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1624,29 +1597,56 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2284,7 +2284,7 @@
   <dimension ref="A2:BQ82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -2363,75 +2363,75 @@
     <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="113"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="35"/>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="97"/>
+      <c r="G7" s="89"/>
       <c r="H7" s="73"/>
     </row>
     <row r="8" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="90"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="36"/>
-      <c r="F8" s="98" t="s">
+      <c r="F8" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="90"/>
+      <c r="G8" s="76"/>
       <c r="H8" s="74" t="str">
         <f>IF(AND($H$7&lt;&gt;"",$D$10&lt;&gt;"",$D$12&lt;&gt;""),_xlfn.XLOOKUP($D$10&amp;$D$12,Apoio!$Y:$Y,Apoio!$Z:$Z)+H7,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="90"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="36"/>
-      <c r="F9" s="99" t="s">
+      <c r="F9" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="100"/>
+      <c r="G9" s="91"/>
       <c r="H9" s="74" t="str">
         <f>IF(AND($H$7&lt;&gt;"",$D$10&lt;&gt;"",$D$12&lt;&gt;""),_xlfn.XLOOKUP($D$10&amp;$D$12,Apoio!$Y:$Y,Apoio!$AA:$AA)+H8,"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="90"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="36"/>
       <c r="E10" s="71"/>
-      <c r="F10" s="110" t="s">
+      <c r="F10" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="111"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="74" t="str">
         <f>IF(AND($H$7&lt;&gt;"",$D$10&lt;&gt;"",$D$12&lt;&gt;""),_xlfn.XLOOKUP($D$10&amp;$D$12,Apoio!$Y:$Y,Apoio!$AB:$AB)+H9,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="90"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="36"/>
     </row>
     <row r="12" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="36"/>
       <c r="F12" s="23"/>
       <c r="G12" s="12" t="s">
@@ -2443,10 +2443,10 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="90"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="36"/>
       <c r="F13" s="24" t="s">
         <v>42</v>
@@ -2457,10 +2457,10 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="90"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="36"/>
       <c r="F14" s="25" t="s">
         <v>44</v>
@@ -2471,10 +2471,10 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="90"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="36"/>
       <c r="F15" s="26" t="s">
         <v>46</v>
@@ -2485,10 +2485,10 @@
       <c r="L15" s="11"/>
     </row>
     <row r="16" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="110" t="s">
+      <c r="B16" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="111"/>
+      <c r="C16" s="102"/>
       <c r="D16" s="37"/>
       <c r="F16" s="59"/>
       <c r="G16" s="59"/>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="17" spans="2:69" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:69" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="97"/>
+      <c r="C18" s="89"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -2510,48 +2510,48 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="2:69" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="101"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="102"/>
-      <c r="F19" s="102"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="103"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="94"/>
     </row>
     <row r="20" spans="2:69" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="104"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="106"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="96"/>
+      <c r="J20" s="97"/>
     </row>
     <row r="21" spans="2:69" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="104"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="105"/>
-      <c r="I21" s="105"/>
-      <c r="J21" s="106"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="96"/>
+      <c r="J21" s="97"/>
     </row>
     <row r="22" spans="2:69" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="107"/>
-      <c r="C22" s="108"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="108"/>
-      <c r="H22" s="108"/>
-      <c r="I22" s="108"/>
-      <c r="J22" s="109"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="100"/>
     </row>
     <row r="23" spans="2:69" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:69" s="16" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6173,13 +6173,13 @@
     </row>
     <row r="47" spans="1:53" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10"/>
-      <c r="B47" s="79" t="s">
+      <c r="B47" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="80"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="80"/>
+      <c r="C47" s="109"/>
+      <c r="D47" s="109"/>
+      <c r="E47" s="109"/>
+      <c r="F47" s="109"/>
       <c r="G47" s="38" t="str">
         <f>IF(F25&lt;&gt;"",IF(ISNUMBER(F25),SUMPRODUCT($F$25:$F$46,$G$25:$G$46),SUM($G$25:$G$46)),"")</f>
         <v/>
@@ -6319,13 +6319,13 @@
       <c r="AW49" s="27"/>
     </row>
     <row r="50" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114" t="s">
+      <c r="B50" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="118" t="s">
+      <c r="C50" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="113"/>
+      <c r="D50" s="85"/>
       <c r="E50" s="20" t="str">
         <f>IF(I47&lt;&gt;0,I47,"")</f>
         <v/>
@@ -6347,11 +6347,11 @@
       <c r="AW50" s="27"/>
     </row>
     <row r="51" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="115"/>
-      <c r="C51" s="89" t="s">
+      <c r="B51" s="81"/>
+      <c r="C51" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="90"/>
+      <c r="D51" s="76"/>
       <c r="E51" s="66" t="e">
         <f>L47*G13</f>
         <v>#VALUE!</v>
@@ -6374,11 +6374,11 @@
       <c r="AW51" s="27"/>
     </row>
     <row r="52" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="115"/>
-      <c r="C52" s="89" t="s">
+      <c r="B52" s="81"/>
+      <c r="C52" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="90"/>
+      <c r="D52" s="76"/>
       <c r="E52" s="5" t="e">
         <f>E50*1.1%</f>
         <v>#VALUE!</v>
@@ -6399,11 +6399,11 @@
       <c r="J52" s="34"/>
     </row>
     <row r="53" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="115"/>
-      <c r="C53" s="116" t="s">
+      <c r="B53" s="81"/>
+      <c r="C53" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="117"/>
+      <c r="D53" s="83"/>
       <c r="E53" s="29" t="e">
         <f>IF(SUM(E50:E52)&lt;&gt;0,SUM(E50:E52),"")</f>
         <v>#VALUE!</v>
@@ -6430,13 +6430,13 @@
       </c>
     </row>
     <row r="54" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="87" t="s">
+      <c r="B54" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="91" t="s">
+      <c r="C54" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="92"/>
+      <c r="D54" s="119"/>
       <c r="E54" s="20" t="str">
         <f>IF(I47&lt;&gt;0,$V$47,"")</f>
         <v/>
@@ -6457,11 +6457,11 @@
       <c r="J54" s="34"/>
     </row>
     <row r="55" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="87"/>
-      <c r="C55" s="89" t="s">
+      <c r="B55" s="116"/>
+      <c r="C55" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="90"/>
+      <c r="D55" s="76"/>
       <c r="E55" s="20" t="str">
         <f>IF(I47&lt;&gt;0,$W$47,"")</f>
         <v/>
@@ -6482,11 +6482,11 @@
       <c r="J55" s="34"/>
     </row>
     <row r="56" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="87"/>
-      <c r="C56" s="89" t="s">
+      <c r="B56" s="116"/>
+      <c r="C56" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="90"/>
+      <c r="D56" s="76"/>
       <c r="E56" s="20" t="str">
         <f>IF(I47&lt;&gt;0,$X$47,"")</f>
         <v/>
@@ -6507,11 +6507,11 @@
       <c r="J56" s="34"/>
     </row>
     <row r="57" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="87"/>
-      <c r="C57" s="89" t="s">
+      <c r="B57" s="116"/>
+      <c r="C57" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="90"/>
+      <c r="D57" s="76"/>
       <c r="E57" s="20" t="str">
         <f>IF(I47&lt;&gt;0,IF($D$13="Revenda",0,$Y$47),"")</f>
         <v/>
@@ -6532,11 +6532,11 @@
       <c r="J57" s="34"/>
     </row>
     <row r="58" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="87"/>
-      <c r="C58" s="89" t="s">
+      <c r="B58" s="116"/>
+      <c r="C58" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="90"/>
+      <c r="D58" s="76"/>
       <c r="E58" s="20" t="str">
         <f>IF(I47&lt;&gt;0,$Z$47,"")</f>
         <v/>
@@ -6557,11 +6557,11 @@
       <c r="J58" s="34"/>
     </row>
     <row r="59" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="88"/>
-      <c r="C59" s="93" t="s">
+      <c r="B59" s="117"/>
+      <c r="C59" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="D59" s="94"/>
+      <c r="D59" s="78"/>
       <c r="E59" s="29" t="str">
         <f>IF(SUM(E54:E58)&lt;&gt;0,SUM(E54:E58),"")</f>
         <v/>
@@ -6588,13 +6588,13 @@
       </c>
     </row>
     <row r="60" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="95" t="s">
+      <c r="B60" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="89" t="s">
+      <c r="C60" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="D60" s="90"/>
+      <c r="D60" s="76"/>
       <c r="E60" s="20" t="str">
         <f>IF(I47&lt;&gt;"",IF(D12="By Air",0,IF(I47&lt;&gt;0,8%*SUM(E51:E52,E64)+21.2/$G$13,"")),"")</f>
         <v/>
@@ -6615,11 +6615,11 @@
       <c r="J60" s="34"/>
     </row>
     <row r="61" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="87"/>
-      <c r="C61" s="89" t="s">
+      <c r="B61" s="116"/>
+      <c r="C61" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="90"/>
+      <c r="D61" s="76"/>
       <c r="E61" s="20" t="str">
         <f>IF(I47&lt;&gt;"",_xlfn.XLOOKUP(COUNTA(_xlfn.UNIQUE(N25:N46))-1,Apoio_Tabela_Siscomex3[Número de NCMs],Apoio_Tabela_Siscomex3[Valor Final])/$G$13,"")</f>
         <v/>
@@ -6640,11 +6640,11 @@
       <c r="J61" s="34"/>
     </row>
     <row r="62" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="87"/>
-      <c r="C62" s="89" t="s">
+      <c r="B62" s="116"/>
+      <c r="C62" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="D62" s="90"/>
+      <c r="D62" s="76"/>
       <c r="E62" s="20" t="str" cm="1">
         <f t="array" ref="E62">IF(I47&lt;&gt;"",IF(D12="Entreposto",0,IF(D12="By Sea",((0.35%+0.05%)*SUM(E50:E52))+(540+660)/$G$13,(_xlfn.IFS($L$47&lt;Apoio!O2,Apoio!Q2,$L$47&lt;Apoio!O3,Apoio!Q3,$L$47&lt;Apoio!O4,Apoio!Q4,$L$47&lt;Apoio!O5,Apoio!Q5,$L$47&lt;Apoio!O6,Apoio!Q6,$L$47&lt;Apoio!O7,Apoio!Q7,$L$47&lt;Apoio!O8,Apoio!Q8,$L$47&lt;Apoio!O9,Apoio!Q9))/$G$13+0.75%*SUM(E50:E52,E65))),"")</f>
         <v/>
@@ -6665,8 +6665,8 @@
       <c r="J62" s="34"/>
     </row>
     <row r="63" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="87"/>
-      <c r="C63" s="119" t="s">
+      <c r="B63" s="116"/>
+      <c r="C63" s="86" t="s">
         <v>58</v>
       </c>
       <c r="D63" s="31" t="s">
@@ -6694,8 +6694,8 @@
       <c r="Q63" s="11"/>
     </row>
     <row r="64" spans="2:49" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="87"/>
-      <c r="C64" s="120"/>
+      <c r="B64" s="116"/>
+      <c r="C64" s="87"/>
       <c r="D64" s="31" t="s">
         <v>33</v>
       </c>
@@ -6721,8 +6721,8 @@
       <c r="Q64" s="11"/>
     </row>
     <row r="65" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="87"/>
-      <c r="C65" s="119" t="s">
+      <c r="B65" s="116"/>
+      <c r="C65" s="86" t="s">
         <v>95</v>
       </c>
       <c r="D65" s="31" t="s">
@@ -6751,8 +6751,8 @@
       <c r="Q65" s="11"/>
     </row>
     <row r="66" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="87"/>
-      <c r="C66" s="120"/>
+      <c r="B66" s="116"/>
+      <c r="C66" s="87"/>
       <c r="D66" s="31" t="s">
         <v>96</v>
       </c>
@@ -6779,11 +6779,11 @@
       <c r="Q66" s="11"/>
     </row>
     <row r="67" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="87"/>
-      <c r="C67" s="89" t="s">
+      <c r="B67" s="116"/>
+      <c r="C67" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="D67" s="90"/>
+      <c r="D67" s="76"/>
       <c r="E67" s="20" t="str">
         <f>IF($I$47&lt;&gt;"",_xlfn.XLOOKUP($D$16,Tabela1[Tradin/Despachante],Tabela1[Custo],0)/$G$13,"")</f>
         <v/>
@@ -6807,11 +6807,11 @@
       <c r="Q67" s="11"/>
     </row>
     <row r="68" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="87"/>
-      <c r="C68" s="89" t="s">
+      <c r="B68" s="116"/>
+      <c r="C68" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="90"/>
+      <c r="D68" s="76"/>
       <c r="E68" s="5">
         <v>0</v>
       </c>
@@ -6834,11 +6834,11 @@
       <c r="Q68" s="11"/>
     </row>
     <row r="69" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="88"/>
-      <c r="C69" s="93" t="s">
+      <c r="B69" s="117"/>
+      <c r="C69" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="D69" s="94"/>
+      <c r="D69" s="78"/>
       <c r="E69" s="29" t="str">
         <f>IF(SUM(E60:E68)&lt;&gt;0,SUM(E60:E68),"")</f>
         <v/>
@@ -6865,13 +6865,13 @@
       </c>
     </row>
     <row r="70" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="95" t="s">
+      <c r="B70" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="C70" s="89" t="s">
+      <c r="C70" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="D70" s="90"/>
+      <c r="D70" s="76"/>
       <c r="E70" s="20" t="str">
         <f>IF(I47&lt;&gt;"",$AO$47,"")</f>
         <v/>
@@ -6892,11 +6892,11 @@
       <c r="J70" s="34"/>
     </row>
     <row r="71" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="88"/>
-      <c r="C71" s="89" t="s">
+      <c r="B71" s="117"/>
+      <c r="C71" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="90"/>
+      <c r="D71" s="76"/>
       <c r="E71" s="20" t="str">
         <f>IF(I47&lt;&gt;"",$AP$47,"")</f>
         <v/>
@@ -6917,11 +6917,11 @@
       <c r="J71" s="34"/>
     </row>
     <row r="72" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="84" t="s">
+      <c r="B72" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="C72" s="85"/>
-      <c r="D72" s="86"/>
+      <c r="C72" s="114"/>
+      <c r="D72" s="115"/>
       <c r="E72" s="29" t="e">
         <f>IF(SUM(E50:E52,E54:E58,E60:E68,E70:E71)&lt;&gt;0,SUM(E50:E52,E54:E58,E60:E68,E70:E71),"")</f>
         <v>#VALUE!</v>
@@ -6967,11 +6967,11 @@
     </row>
     <row r="74" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="81" t="s">
+      <c r="B75" s="110" t="s">
         <v>60</v>
       </c>
-      <c r="C75" s="82"/>
-      <c r="D75" s="83"/>
+      <c r="C75" s="111"/>
+      <c r="D75" s="112"/>
       <c r="E75" s="20" t="str">
         <f>IFERROR(E70*_xlfn.XLOOKUP($D$16,Tabela1[Tradin/Despachante],Tabela1[Bonificação]),"")</f>
         <v/>
@@ -6998,11 +6998,11 @@
       </c>
     </row>
     <row r="76" spans="2:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="81" t="s">
+      <c r="B76" s="110" t="s">
         <v>61</v>
       </c>
-      <c r="C76" s="82"/>
-      <c r="D76" s="83"/>
+      <c r="C76" s="111"/>
+      <c r="D76" s="112"/>
       <c r="E76" s="21" t="str">
         <f t="shared" ref="E76:G76" si="58">IFERROR(IF($D$12="Entreposto",SUM(E70,E60:E68,E54:E58)-E75-E64,IF(OR($D$11="EXW",$D$11="FCA"),SUM(E70,E60:E68,E54:E58,E51:E52)-E75,SUM(E70,E71,E60:E68,E54:E58)-E75)),"")</f>
         <v/>
@@ -7054,10 +7054,10 @@
       </c>
     </row>
     <row r="81" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="77" t="s">
+      <c r="B81" s="106" t="s">
         <v>109</v>
       </c>
-      <c r="C81" s="75" t="s">
+      <c r="C81" s="104" t="s">
         <v>58</v>
       </c>
       <c r="D81" s="56" t="s">
@@ -7069,8 +7069,8 @@
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="78"/>
-      <c r="C82" s="76"/>
+      <c r="B82" s="107"/>
+      <c r="C82" s="105"/>
       <c r="D82" s="57" t="s">
         <v>33</v>
       </c>
@@ -7082,20 +7082,22 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="46">
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B60:B69"/>
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
@@ -7112,22 +7114,20 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B54:B59"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B60:B69"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:C64"/>
   </mergeCells>
   <conditionalFormatting sqref="D7">
     <cfRule type="expression" dxfId="20" priority="24">
@@ -8465,6 +8465,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12124fb0-887f-4a71-9c5c-0b6cc077f367">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d2d8eab5-f6b2-427c-90e3-06dcd0c3f093" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010044C34F8DB67CC4408EAB48300D4F5F36" ma:contentTypeVersion="15" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c400d56ce5c78bcdf0d7fa9db9b4ff3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12124fb0-887f-4a71-9c5c-0b6cc077f367" xmlns:ns3="d2d8eab5-f6b2-427c-90e3-06dcd0c3f093" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="684a882321cfdc22999aa06e0649fb1e" ns2:_="" ns3:_="">
     <xsd:import namespace="12124fb0-887f-4a71-9c5c-0b6cc077f367"/>
@@ -8699,17 +8710,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12124fb0-887f-4a71-9c5c-0b6cc077f367">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d2d8eab5-f6b2-427c-90e3-06dcd0c3f093" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8720,6 +8720,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A075EF4-4D93-4D92-B267-43C46D793769}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12124fb0-887f-4a71-9c5c-0b6cc077f367"/>
+    <ds:schemaRef ds:uri="d2d8eab5-f6b2-427c-90e3-06dcd0c3f093"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AA8F9CF-DEFC-4D0C-9F5B-00629BCB52B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8738,17 +8749,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A075EF4-4D93-4D92-B267-43C46D793769}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12124fb0-887f-4a71-9c5c-0b6cc077f367"/>
-    <ds:schemaRef ds:uri="d2d8eab5-f6b2-427c-90e3-06dcd0c3f093"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64713961-3301-47C5-B011-1730E620963E}">
   <ds:schemaRefs>

</xml_diff>